<commit_message>
Starting to get all the parameter estimate approaches set.  2 down, 2 to go. :)
</commit_message>
<xml_diff>
--- a/data-raw/incubation-model-param.xlsx
+++ b/data-raw/incubation-model-param.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zobitz/Desktop/Fulbright/param-values/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zobitz/Desktop/CanadaFire/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F107A1-83C1-A843-820C-8710574A19CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D82E0D75-A93E-4944-AFE4-770676B3DB1B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="16240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="incubation" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="36">
   <si>
     <t>name</t>
   </si>
@@ -117,17 +117,26 @@
     <t>value</t>
   </si>
   <si>
-    <t>scale_rh</t>
-  </si>
-  <si>
     <t>Scaling factor for fluxes</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g C m^-2 day-1</t>
+  </si>
+  <si>
+    <t>gR</t>
+  </si>
+  <si>
+    <t>Base autotrophic respiration rate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -258,13 +267,6 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -611,10 +613,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -970,10 +971,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1213,13 +1214,13 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" t="s">
         <v>10</v>
       </c>
       <c r="D10" t="b">
@@ -1235,6 +1236,32 @@
         <v>0</v>
       </c>
       <c r="H10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1245,10 +1272,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1489,10 +1516,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
         <v>31</v>
-      </c>
-      <c r="B10" t="s">
-        <v>32</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
@@ -1510,6 +1537,32 @@
         <v>0</v>
       </c>
       <c r="H10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1520,10 +1573,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A11" sqref="A11:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1713,10 +1766,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
         <v>31</v>
-      </c>
-      <c r="B10" t="s">
-        <v>32</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
@@ -1725,10 +1778,30 @@
         <v>1</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="1">
-        <v>100000000</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Oops - forgot these files.
</commit_message>
<xml_diff>
--- a/data-raw/incubation-model-param.xlsx
+++ b/data-raw/incubation-model-param.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zobitz/Desktop/CanadaFire/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zobitz/Desktop/CanadaChronoFire/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D82E0D75-A93E-4944-AFE4-770676B3DB1B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B558E41C-2CE2-7043-A4EA-DE8A905EEE58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="16240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="incubation" sheetId="2" r:id="rId1"/>
@@ -973,8 +973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1275,7 +1275,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:B11"/>
+      <selection activeCell="A12" sqref="A12:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1575,8 +1575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1681,7 +1681,7 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0.01</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1778,10 +1778,10 @@
         <v>1</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F10" s="1">
-        <v>10</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1795,13 +1795,13 @@
         <v>33</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11">
-        <v>10</v>
+        <v>0.01</v>
       </c>
     </row>
   </sheetData>

</xml_diff>